<commit_message>
renaming points or lines into shapes
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1338,7 +1338,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>lines</t>
+          <t>shapes</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1379,7 +1379,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>centroids</t>
+          <t>shapes</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">

</xml_diff>

<commit_message>
Inlining FI output tables and images deployed
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1973,6 +1973,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>table_url</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1984,15 +2025,96 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>df</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source_uri</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2003,7 +2125,589 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_threshold</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>intensity_map_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>profile_rois</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>corner_rois</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_of_illumination</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AI1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nb_pixels_center</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>decile_0</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>decile_1</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>decile_2</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>decile_3</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>decile_4</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>decile_5</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>decile_6</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>decile_7</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>decile_8</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>decile_9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_spots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot_roi</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot_roi</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_intensity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_mean_intensity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_mean_intensity</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>min_max_intensity_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>axis</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measured_band</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2020,781 +2724,82 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>source_uri</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>peak_position_A</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>experimenter</t>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>acquisition_datetime</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>processed</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>processing_datetime</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>field_illumination_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_threshold</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>corner_fraction</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_map</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>profile_rois</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>corner_rois</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_of_illumination</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AI1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nb_pixels_center</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>decile_0</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>decile_1</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>decile_2</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>decile_3</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>decile_4</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>decile_5</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>decile_6</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>decile_7</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>decile_8</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>decile_9</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_spots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot_roi</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot_roi</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_intensity</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_intensity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_mean_intensity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_mean_intensity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>min_max_intensity_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Inlining shapes in rois as dictionaries. labels are identifiers
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -45,6 +45,9 @@
     <sheet name="FieldIlluminationInput" sheetId="36" state="visible" r:id="rId36"/>
     <sheet name="FieldIlluminationOutput" sheetId="37" state="visible" r:id="rId37"/>
     <sheet name="FieldIlluminationKeyValues" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="RoiProfiles" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="RoiCorners" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="RoiCenters" sheetId="41" state="visible" r:id="rId41"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2428,6 +2431,47 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>shapes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -2504,6 +2548,88 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>shapes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>shapes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Added tests for PSF beads. Tested and deployed
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -45,10 +45,14 @@
     <sheet name="RoiMeasurements" sheetId="36" state="visible" r:id="rId36"/>
     <sheet name="TableAsPandasDF" sheetId="37" state="visible" r:id="rId37"/>
     <sheet name="Column" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="FieldIlluminationDataset" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="FieldIlluminationInput" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="FieldIlluminationOutput" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="FieldIlluminationKeyValues" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="PSFBeadsDataset" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="PSFBeadsInput" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="PSFBeadsOutput" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="PSFBeadsKeyMeasurements" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="FieldIlluminationDataset" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="FieldIlluminationInput" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="FieldIlluminationOutput" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="FieldIlluminationKeyValues" sheetId="46" state="visible" r:id="rId46"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2375,6 +2379,420 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>psf_beads_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>min_lateral_distance_factor</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_crops</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centroids</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_axial_edge</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_self_proximity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_cluster</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>psf_properties</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>psf_z_profiles</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>psf_y_profiles</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>psf_x_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AJ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_analyzed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_axial_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_cluster</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_mean</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_median</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_stdev</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_stdev</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_stdev</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2425,7 +2843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2476,7 +2894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Renamed some outputs and changed descriptions
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2379,6 +2379,486 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>min_lateral_distance_factor</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>fitting_rss_threshold</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>intensity_zscore_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_crops</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centroids</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_axial_edge</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_cluster</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>psf_properties</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>psf_z_profiles</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>psf_y_profiles</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>psf_x_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AJ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_analyzed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_axial_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_cluster</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_mean</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_median</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_stdev</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_stdev</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_stdev</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_threshold</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>intensity_map_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2390,41 +2870,308 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>psf_beads_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>profile_rois</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>sigma_x</t>
+          <t>corner_rois</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>center_of_illumination</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AI1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nb_pixels_center</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>decile_0</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>decile_1</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>decile_2</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>decile_3</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>decile_4</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>decile_5</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>decile_6</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>decile_7</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>decile_8</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>decile_9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2441,956 +3188,219 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>bead_crops</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centroids</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_lateral_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_axial_edge</t>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>discarded_bead_centroids_self_proximity</t>
+          <t>experimenter</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>discarded_bead_centroids_cluster</t>
+          <t>acquisition_datetime</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>discarded_bead_centroids_fit_quality</t>
+          <t>processed</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>key_values</t>
+          <t>processing_datetime</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>psf_properties</t>
+          <t>processing_log</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>psf_z_profiles</t>
+          <t>comment</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>psf_y_profiles</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>psf_x_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AJ1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_analyzed</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_axial_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_cluster</t>
+          <t>measured_band</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_fit_quality</t>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_pixels</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_microns</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>peak_position_A</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>fit_quality_z_mean</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>fit_quality_z_median</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>fit_quality_z_stdev</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>fit_quality_y_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>fit_quality_y_median</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>fit_quality_y_stdev</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>fit_quality_x_mean</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>fit_quality_x_median</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>fit_quality_x_stdev</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>field_illumination_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_threshold</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>corner_fraction</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_map</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>profile_rois</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>corner_rois</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_of_illumination</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AI1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nb_pixels_center</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>decile_0</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>decile_1</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>decile_2</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>decile_3</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>decile_4</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>decile_5</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>decile_6</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>decile_7</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>decile_8</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>decile_9</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_pixels</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_microns</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Renamed psf to bead in some instances
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2390,7 +2390,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>psf_beads_images</t>
+          <t>psf_bead_images</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2491,22 +2491,22 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>psf_properties</t>
+          <t>bead_properties</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>psf_z_profiles</t>
+          <t>bead_z_profiles</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>psf_y_profiles</t>
+          <t>bead_y_profiles</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>psf_x_profiles</t>
+          <t>bead_x_profiles</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added saturation threshold and bit-depth to PSF beads input of psf_beads_images
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2379,7 +2379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2395,46 +2395,338 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>min_lateral_distance_factor</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>sigma_z</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>sigma_y</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fitting_rss_threshold</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>intensity_zscore_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_crops</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centroids</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_self_proximity</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>sigma_x</t>
+          <t>considered_bead_centroids_axial_edge</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>snr_threshold</t>
+          <t>considered_bead_centroids_cluster</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>fitting_rss_threshold</t>
+          <t>considered_bead_centroids_fit_quality</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>intensity_zscore_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bead_z_profiles</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_y_profiles</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_x_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AJ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_analyzed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_axial_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_cluster</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_mean</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_median</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fit_quality_z_stdev</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>fit_quality_y_stdev</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>fit_quality_x_stdev</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>resolution_stdev_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2451,956 +2743,674 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>bead_crops</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centroids</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_lateral_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_self_proximity</t>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>considered_bead_centroids_axial_edge</t>
+          <t>experimenter</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>considered_bead_centroids_cluster</t>
+          <t>acquisition_datetime</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>considered_bead_centroids_fit_quality</t>
+          <t>processed</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_threshold</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>intensity_map_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>key_values</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>profile_rois</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>corner_rois</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_of_illumination</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AI1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nb_pixels_center</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>bead_properties</t>
+          <t>top_left_intensity_ratio</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>bead_z_profiles</t>
+          <t>top_center_intensity_mean</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>bead_y_profiles</t>
+          <t>top_center_intensity_ratio</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>bead_x_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AJ1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_analyzed</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_axial_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>decile_0</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>decile_1</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>decile_2</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>decile_3</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>decile_4</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>decile_5</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>decile_6</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>decile_7</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>decile_8</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>decile_9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_cluster</t>
+          <t>std_3d_dist</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_fit_quality</t>
+          <t>mad_3d_dist</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>fit_quality_z_mean</t>
+          <t>mean_z_dist</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>fit_quality_z_median</t>
+          <t>median_z_dist</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>fit_quality_z_stdev</t>
+          <t>std_z_dist</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>fit_quality_y_mean</t>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>fit_quality_y_median</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>fit_quality_y_stdev</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>fit_quality_x_mean</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>fit_quality_x_median</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>fit_quality_x_stdev</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>resolution_stdev_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>experimenter</t>
+          <t>measured_band</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>acquisition_datetime</t>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_pixels</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_microns</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>peak_position_A</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>processed</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>processing_datetime</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>processing_log</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>field_illumination_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_threshold</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>corner_fraction</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_map</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>profile_rois</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>corner_rois</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_of_illumination</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AI1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nb_pixels_center</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>decile_0</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>decile_1</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>decile_2</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>decile_3</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>decile_4</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>decile_5</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>decile_6</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>decile_7</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>decile_8</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>decile_9</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_pixels</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_microns</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Changed naming of center of mass to centroid weighted and added centroid (geometric
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2920,7 +2920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2941,176 +2941,425 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
+          <t>centroid_weighted_y</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>centroid_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>centroid_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>max_intensity</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>decile_0</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>decile_1</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>decile_2</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>decile_3</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>decile_4</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>decile_5</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>decile_6</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>decile_7</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>decile_8</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>decile_9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_x</t>
+          <t>mad_3d_dist</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_y</t>
+          <t>mean_z_dist</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>top_left_intensity_mean</t>
+          <t>median_z_dist</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>top_left_intensity_ratio</t>
+          <t>std_z_dist</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>top_center_intensity_mean</t>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>top_center_intensity_ratio</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>decile_0</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>decile_1</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>decile_2</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>decile_3</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>decile_4</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>decile_5</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>decile_6</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>decile_7</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>decile_8</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>decile_9</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measured_band</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3127,290 +3376,51 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_pixels</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_microns</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>std_3d_dist</t>
+          <t>peak_position_A</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>mad_3d_dist</t>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>mean_z_dist</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>median_z_dist</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>std_z_dist</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_pixels</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_microns</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Many changes into field illumination schema - removed input param center threshold - renamed rois to start with ROI - refactored centroids to add relative positions and relative distances in 2d
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2813,7 +2813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2839,31 +2839,510 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>center_threshold</t>
+          <t>corner_fraction</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>corner_fraction</t>
+          <t>sigma</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>sigma</t>
+          <t>intensity_map_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centroids_weighted</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AZ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y_relative</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>centroid_weighted_x_relative</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_distance_relative</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>centroid_y</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>centroid_y_relative</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>centroid_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>centroid_x_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>centroid_distance_relative</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_y</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_x</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>decile_0</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>decile_1</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>decile_2</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>decile_3</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>decile_4</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>decile_5</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>decile_6</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>decile_7</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>decile_8</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>decile_9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2880,547 +3359,138 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measured_band</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>intensity_profiles</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_map</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>profile_rois</t>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_pixels</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_microns</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>corner_rois</t>
+          <t>peak_position_A</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>center_of_illumination</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AK1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>center_fraction</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_y</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_x</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>centroid_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>centroid_x</t>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>max_intensity</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_x</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_y</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>decile_0</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>decile_1</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>decile_2</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>decile_3</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>decile_4</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>decile_5</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>decile_6</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>decile_7</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>decile_8</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>decile_9</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_pixels</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_microns</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Refactored psf beads changed channel to channel_nr
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2314,7 +2314,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>channel_nr</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2531,202 +2531,702 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>nr_of_beads_analyzed</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>nr_of_beads_discarded_lateral_edge</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>nr_of_beads_discarded_axial_edge</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>nr_of_beads_discarded_self_proximity</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_z_fit</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_y_fit</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_x_fit</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_std</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_std</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_median</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_std</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_cluster</t>
+          <t>experimenter</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_fit_quality</t>
+          <t>acquisition_datetime</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>fit_quality_z_mean</t>
+          <t>processed</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>fit_quality_z_median</t>
+          <t>processing_datetime</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>fit_quality_z_stdev</t>
+          <t>processing_log</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>fit_quality_y_mean</t>
+          <t>comment</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>fit_quality_y_median</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>fit_quality_y_stdev</t>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_map_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centroids_weighted</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y_relative</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x_relative</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_distance_relative</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>centroid_y</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>centroid_y_relative</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>centroid_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>centroid_x_relative</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>fit_quality_x_mean</t>
+          <t>centroid_distance_relative</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>fit_quality_x_median</t>
+          <t>centroid_fitted_y</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>fit_quality_x_stdev</t>
+          <t>centroid_fitted_y_relative</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_z_pixels</t>
+          <t>centroid_fitted_x</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_z_pixels</t>
+          <t>centroid_fitted_x_relative</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>resolution_stdev_fwhm_z_pixels</t>
+          <t>centroid_fitted_distance_relative</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_y_pixels</t>
+          <t>max_intensity</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_y_pixels</t>
+          <t>max_intensity_pos_y</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>resolution_stdev_fwhm_y_pixels</t>
+          <t>max_intensity_pos_y_relative</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_x_pixels</t>
+          <t>max_intensity_pos_x</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_x_pixels</t>
+          <t>max_intensity_pos_x_relative</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>resolution_stdev_fwhm_x_pixels</t>
+          <t>max_intensity_distance_relative</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_z_microns</t>
+          <t>top_left_intensity_mean</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_z_microns</t>
+          <t>top_left_intensity_ratio</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>resolution_stdev_fwhm_z_microns</t>
+          <t>top_center_intensity_mean</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_y_microns</t>
+          <t>top_center_intensity_ratio</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_y_microns</t>
+          <t>top_right_intensity_mean</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>resolution_stdev_fwhm_y_microns</t>
+          <t>top_right_intensity_ratio</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_x_microns</t>
+          <t>middle_left_intensity_mean</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_x_microns</t>
+          <t>middle_left_intensity_ratio</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>resolution_stdev_fwhm_x_microns</t>
+          <t>middle_center_intensity_mean</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+          <t>middle_center_intensity_ratio</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+          <t>middle_right_intensity_mean</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>resolution_stdev_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2807,7 +3307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2824,7 +3324,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>field_illumination_image</t>
+          <t>argolight_e_image</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2839,608 +3339,123 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>corner_fraction</t>
+          <t>orientation_axis</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>sigma</t>
+          <t>measured_band</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>intensity_profiles</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_map</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>roi_profiles</t>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_pixels</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_microns</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>roi_corners</t>
+          <t>peak_position_A</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>roi_centroids_weighted</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AP1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_y_relative</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_x</t>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>centroid_weighted_x_relative</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>centroid_weighted_distance_relative</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>centroid_y</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>centroid_y_relative</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>centroid_x</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>centroid_x_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>centroid_distance_relative</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_y</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_x</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_pixels</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_microns</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Fixing error with axial edge beads named discarded instead of considered
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2557,12 +2557,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_axial_edge</t>
+          <t>nr_of_beads_discarded_self_proximity</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
+          <t>nr_of_beads_considered_axial_edge</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">

</xml_diff>

<commit_message>
Split bead fit quality beads into z, y and x
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2450,6 +2450,313 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_crops</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centroids</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_axial_edge</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_z_profiles</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_y_profiles</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>bead_x_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_analyzed</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_axial_edge</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_z_fit</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_y_fit</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_x_fit</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_std</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_std</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_median</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_std</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2461,77 +2768,649 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>bead_crops</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centroids</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_lateral_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_self_proximity</t>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>considered_bead_centroids_axial_edge</t>
+          <t>experimenter</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>considered_bead_centroids_intensity_outlier</t>
+          <t>acquisition_datetime</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>considered_bead_centroids_fit_quality</t>
+          <t>processed</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_map_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>key_values</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centroids_weighted</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y_relative</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x_relative</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_distance_relative</t>
+        </is>
+      </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>bead_properties</t>
+          <t>centroid_y</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>bead_z_profiles</t>
+          <t>centroid_y_relative</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>bead_y_profiles</t>
+          <t>centroid_x</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>bead_x_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AM1"/>
+          <t>centroid_x_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>centroid_distance_relative</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_y</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_x</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measured_band</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2547,915 +3426,46 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>nr_of_beads_analyzed</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_lateral_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_pixels</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_microns</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_axial_edge</t>
+          <t>peak_position_A</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_intensity_outlier</t>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_bad_z_fit</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_bad_y_fit</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_bad_x_fit</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>fit_rss_z_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>fit_rss_z_median</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>fit_rss_z_std</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>fit_rss_y_mean</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>fit_rss_y_median</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>fit_rss_y_std</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>fit_rss_x_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>fit_rss_x_median</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>fit_rss_x_std</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>field_illumination_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>corner_fraction</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_map</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>roi_profiles</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>roi_corners</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>roi_centroids_weighted</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AP1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_y_relative</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_x_relative</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_distance_relative</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>centroid_y</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>centroid_y_relative</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>centroid_x</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>centroid_x_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>centroid_distance_relative</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_y</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_x</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_pixels</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_microns</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Minor changes to column class: - added description to the column - Values are not required. That allows us to  create empty tables
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2186,6 +2186,1199 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>source_uri</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_spots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot_roi</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot_roi</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_intensity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_mean_intensity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_mean_intensity</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>min_max_intensity_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>min_lateral_distance_factor</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fitting_rss_threshold</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>intensity_zscore_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_crops</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centroids</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centroids_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_axial_edge</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>considered_bead_centroids_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_z_profiles</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_y_profiles</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>bead_x_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_analyzed</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_axial_edge</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_z_fit</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_y_fit</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_x_fit</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>fit_rss_z_std</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>fit_rss_y_std</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_median</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fit_rss_x_std</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_map_size</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_map</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centroids_weighted</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AP1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_y_relative</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_x_relative</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>centroid_weighted_distance_relative</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>centroid_y</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>centroid_y_relative</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>centroid_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>centroid_x_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>centroid_distance_relative</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_y</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_x</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>centroid_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measured_band</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2197,1275 +3390,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>source_uri</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>focus_slice</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_pixels</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rayleigh_resolution_microns</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>experimenter</t>
+          <t>peak_position_A</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>acquisition_datetime</t>
+          <t>peak_position_B</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>processed</t>
+          <t>peak_height_A</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>processing_datetime</t>
+          <t>peak_height_B</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>processing_log</t>
+          <t>peak_prominence_A</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_spots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot_roi</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot_roi</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_intensity</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_intensity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_mean_intensity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_mean_intensity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>min_max_intensity_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fitting_rss_threshold</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>intensity_zscore_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bead_crops</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centroids</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_lateral_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centroids_self_proximity</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_bead_centroids_axial_edge</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_bead_centroids_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bead_centroids_z_fit_quality</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bead_centroids_y_fit_quality</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>considered_bead_centroids_x_fit_quality</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>bead_properties</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>bead_z_profiles</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>bead_y_profiles</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>bead_x_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AM1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_analyzed</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_lateral_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_axial_edge</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_bad_z_fit</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_bad_y_fit</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_bad_x_fit</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>fit_rss_z_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>fit_rss_z_median</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>fit_rss_z_std</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>fit_rss_y_mean</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>fit_rss_y_median</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>fit_rss_y_std</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>fit_rss_x_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>fit_rss_x_median</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>fit_rss_x_std</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>field_illumination_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>corner_fraction</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_map</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>roi_profiles</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>roi_corners</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>roi_centroids_weighted</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AP1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_y_relative</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_x_relative</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>centroid_weighted_distance_relative</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>centroid_y</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>centroid_y_relative</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>centroid_x</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>centroid_x_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>centroid_distance_relative</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_y</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_x</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>centroid_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>focus_slice</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_pixels</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>rayleigh_resolution_microns</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>peak_position_A</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>peak_position_B</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>peak_height_A</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>peak_height_B</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>peak_prominence_A</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>peak_prominence_B</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Added author to comments
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -746,7 +746,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -762,10 +762,15 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>author</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>comment_type</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>text</t>
         </is>
@@ -773,7 +778,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"ACQUISITION,PROCESSING,OTHER"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Making thins not inlined Fixing strategies errors in outlining Not all tests passing
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1878,7 +1878,7 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>comments</t>
         </is>
       </c>
     </row>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>comments</t>
         </is>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>comments</t>
         </is>
       </c>
     </row>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>comments</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some errors. Going home
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1878,7 +1878,7 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>comments</t>
+          <t>comment</t>
         </is>
       </c>
     </row>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>comments</t>
+          <t>comment</t>
         </is>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>comments</t>
+          <t>comment</t>
         </is>
       </c>
     </row>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>comments</t>
+          <t>comment</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Source_image inlined and renamed to plural
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1304,7 +1304,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>source_image</t>
+          <t>source_images</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
@@ -1430,7 +1430,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>source_image</t>
+          <t>source_images</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">

</xml_diff>

<commit_message>
Moved things from slots to attributes Added image acquisition date time
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1295,7 +1295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1356,50 +1356,55 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>source_images</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>array_data</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>data_uri</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>omero_host</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>omero_port</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>omero_object_type</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>omero_object_id</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>linked_objects</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1407,7 +1412,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"IMAGE,DATASET,PROJECT,GROUP,TABLE,KEY_VALUES,ROI"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1421,7 +1426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1482,50 +1487,55 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>source_images</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>array_data</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>data_uri</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>omero_host</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>omero_port</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>omero_object_type</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>omero_object_id</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>linked_objects</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1533,7 +1543,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"IMAGE,DATASET,PROJECT,GROUP,TABLE,KEY_VALUES,ROI"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Rename all RSS to R2 for coefficient of determination deployed and tests passing
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -681,7 +681,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"IMAGE,DATASET,PROJECT,GROUP,EXPERIMENTER,TABLE,KEY_VALUES,TAG,COMMENT,ROI,FILE"</formula1>
+      <formula1>"IMAGE,DATASET,PROJECT,EXPERIMENTERGROUP,EXPERIMENTER,TABLE,KEY_VALUES,TAG,COMMENT,ROI,FILE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>fitting_rss_threshold</t>
+          <t>fitting_r2_threshold</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -2717,47 +2717,47 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>fit_rss_z_mean</t>
+          <t>fit_r2_z_mean</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>fit_rss_z_median</t>
+          <t>fit_r2_z_median</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>fit_rss_z_std</t>
+          <t>fit_r2_z_std</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>fit_rss_y_mean</t>
+          <t>fit_r2_y_mean</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>fit_rss_y_median</t>
+          <t>fit_r2_y_median</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>fit_rss_y_std</t>
+          <t>fit_r2_y_std</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>fit_rss_x_mean</t>
+          <t>fit_r2_x_mean</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>fit_rss_x_median</t>
+          <t>fit_r2_x_median</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>fit_rss_x_std</t>
+          <t>fit_r2_x_std</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">

</xml_diff>

<commit_message>
Removed low res intensity map. To be replaced with a mask ROI
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2973,6 +2973,672 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_values</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_maps</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centers_of_mass</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>roi_centers_geometric</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>roi_centers_fitted</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>roi_centers_max_intensity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AT1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y_relative</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x_relative</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>center_of_mass_distance_relative</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>center_geometric_y</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>center_geometric_y_relative</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>center_geometric_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>center_geometric_x_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>center_geometric_distance_relative</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>center_fitted_y</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>center_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>center_fitted_x</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>center_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>center_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_spots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot_roi</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot_roi</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_intensity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_mean_intensity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_mean_intensity</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>min_max_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2984,7 +3650,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>field_illumination_image</t>
+          <t>argolight_e_image</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2999,122 +3665,92 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>corner_fraction</t>
+          <t>orientation_axis</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>sigma</t>
+          <t>measured_band</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>intensity_map_size</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>intensity_profiles</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_maps</t>
-        </is>
-      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>roi_profiles</t>
+          <t>processing_application</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>roi_corners</t>
+          <t>processing_version</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>roi_centers_of_mass</t>
+          <t>processing_entity</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>roi_centers_geometric</t>
+          <t>processing_datetime</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>roi_centers_fitted</t>
+          <t>processing_log</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>roi_centers_max_intensity</t>
+          <t>warnings</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>processing_application</t>
+          <t>errors</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
           <t>comment</t>
         </is>
       </c>
@@ -3122,645 +3758,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AT1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y_relative</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x_relative</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>center_of_mass_distance_relative</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>center_geometric_y</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>center_geometric_y_relative</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>center_geometric_x</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>center_geometric_x_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>center_geometric_distance_relative</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>center_fitted_y</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>center_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>center_fitted_x</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>center_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>center_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_spots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot_roi</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot_roi</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_intensity</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_intensity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_mean_intensity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_mean_intensity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>min_max_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added roi_center_region as a mask ROI.
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -3019,7 +3019,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3075,40 +3075,686 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>roi_center_region</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>processing_application</t>
         </is>
       </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AT1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y_relative</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x_relative</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>center_of_mass_distance_relative</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>center_geometric_y</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>center_geometric_y_relative</t>
+        </is>
+      </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>center_geometric_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>center_geometric_x_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>center_geometric_distance_relative</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>center_fitted_y</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>center_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>center_fitted_x</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>center_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>center_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_spots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot_roi</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot_roi</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_intensity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_mean_intensity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_mean_intensity</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>min_max_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measured_band</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>processing_version</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>processing_entity</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>processing_datetime</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>processing_log</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>warnings</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>errors</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
@@ -3117,645 +3763,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AT1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y_relative</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x_relative</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>center_of_mass_distance_relative</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>center_geometric_y</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>center_geometric_y_relative</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>center_geometric_x</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>center_geometric_x_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>center_geometric_distance_relative</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>center_fitted_y</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>center_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>center_fitted_x</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>center_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>center_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_spots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot_roi</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot_roi</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_intensity</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_intensity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_mean_intensity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_mean_intensity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>min_max_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed bead crops from PSFBeadsOutput
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2530,121 +2530,1221 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bead_crops</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>analyzed_bead_centers</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>discarded_bead_centers_lateral_edge</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>discarded_bead_centers_self_proximity</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>discarded_bead_centers_self_proximity</t>
+          <t>considered_bead_centers_axial_edge</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>considered_bead_centers_axial_edge</t>
+          <t>considered_bead_centers_intensity_outlier</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>considered_bead_centers_intensity_outlier</t>
+          <t>considered_bead_centers_z_fit_quality</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>considered_bead_centers_z_fit_quality</t>
+          <t>considered_bead_centers_y_fit_quality</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>considered_bead_centers_y_fit_quality</t>
+          <t>considered_bead_centers_x_fit_quality</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>considered_bead_centers_x_fit_quality</t>
+          <t>key_values</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_z_profiles</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_y_profiles</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_x_profiles</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AQ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_analyzed</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_lateral_edge</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_discarded_self_proximity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_axial_edge</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_z_fit</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_y_fit</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>nr_of_beads_considered_bad_x_fit</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_std</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_std</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_median</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_std</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_pixels</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_pixels</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_pixels</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_z_microns</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_y_microns</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_x_microns</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>key_values</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>roi_centers_of_mass</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centers_geometric</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>roi_centers_fitted</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>roi_centers_max_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>roi_center_region</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>bead_properties</t>
+          <t>processing_version</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>bead_z_profiles</t>
+          <t>processing_entity</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>bead_y_profiles</t>
+          <t>processing_datetime</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>bead_x_profiles</t>
+          <t>processing_log</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AT1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y_relative</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x_relative</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>center_of_mass_distance_relative</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>center_geometric_y</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>center_geometric_y_relative</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>center_geometric_x</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>center_geometric_x_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>center_geometric_distance_relative</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>center_fitted_y</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>center_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>center_fitted_x</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>center_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>center_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nr_of_spots</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>intensity_max_spot_roi</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>intensity_min_spot_roi</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_intensity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_mean_intensity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_mean_intensity</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>min_max_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mean_3d_dist</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>median_3d_dist</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>std_3d_dist</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>mad_3d_dist</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mean_z_dist</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>median_z_dist</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>std_z_dist</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mad_z_dist</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_e_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>orientation_axis</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>measured_band</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prominence_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>peaks_rois</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>processing_application</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>processing_version</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>processing_entity</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>processing_datetime</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>processing_log</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>warnings</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>errors</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
@@ -2653,1109 +3753,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AQ1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_analyzed</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_lateral_edge</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_axial_edge</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_bad_z_fit</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_bad_y_fit</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>nr_of_beads_considered_bad_x_fit</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_median</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_std</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_mean</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_median</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_std</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_median</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_std</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_z_microns</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_y_microns</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_x_microns</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>field_illumination_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>corner_fraction</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_values</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>roi_profiles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>roi_corners</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>roi_centers_of_mass</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>roi_centers_geometric</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>roi_centers_fitted</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>roi_centers_max_intensity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>roi_center_region</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AT1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y_relative</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x_relative</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>center_of_mass_distance_relative</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>center_geometric_y</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>center_geometric_y_relative</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>center_geometric_x</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>center_geometric_x_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>center_geometric_distance_relative</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>center_fitted_y</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>center_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>center_fitted_x</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>center_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>center_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nr_of_spots</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>intensity_max_spot_roi</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>intensity_min_spot_roi</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_intensity</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_intensity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_mean_intensity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_mean_intensity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>min_max_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_A</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_B</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mean_3d_dist</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>median_3d_dist</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>std_3d_dist</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>mad_3d_dist</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>mean_z_dist</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>median_z_dist</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>std_z_dist</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>mad_z_dist</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_e_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>orientation_axis</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>measured_band</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>prominence_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>peaks_rois</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Making image acquisition_datetime optional
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1824,7 +1824,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1915,6 +1915,16 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>comment</t>
         </is>
       </c>
@@ -2328,7 +2338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2439,6 +2449,16 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>comment</t>
         </is>
       </c>
@@ -2837,7 +2857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2912,6 +2932,16 @@
         </is>
       </c>
       <c r="N1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
@@ -3384,7 +3414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3444,6 +3474,16 @@
         </is>
       </c>
       <c r="K1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
         <is>
           <t>comment</t>
         </is>

</xml_diff>

<commit_message>
Renamed beads from "discarded" to "considered"
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2354,12 +2354,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>discarded_bead_centers_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>discarded_bead_centers_self_proximity</t>
+          <t>considered_bead_centers_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_self_proximity</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -2495,12 +2495,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_lateral_edge</t>
+          <t>nr_of_beads_considered_lateral_edge</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
+          <t>nr_of_beads_considered_self_proximity</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">

</xml_diff>

<commit_message>
Refactored psf_beads_schema.yaml. Added KeyMeasurements as a table to store those as a table
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -42,7 +42,7 @@
     <sheet name="PSFBeadsDataset" sheetId="33" state="visible" r:id="rId33"/>
     <sheet name="PSFBeadsInput" sheetId="34" state="visible" r:id="rId34"/>
     <sheet name="PSFBeadsOutput" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="PSFBeadsKeyValues" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="PSFBeadsKeyMeasurements" sheetId="36" state="visible" r:id="rId36"/>
     <sheet name="ArgolightBDataset" sheetId="37" state="visible" r:id="rId37"/>
     <sheet name="ArgolightBInput" sheetId="38" state="visible" r:id="rId38"/>
     <sheet name="ArgolightBOutput" sheetId="39" state="visible" r:id="rId39"/>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>key_values</t>
+          <t>key_measurements</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -2474,7 +2474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:BB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2490,210 +2490,265 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>nr_of_beads_analyzed</t>
+          <t>considered_valid_count</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_lateral_edge</t>
+          <t>considered_self_proximity_count</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>nr_of_beads_discarded_self_proximity</t>
+          <t>considered_lateral_edge_count</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_axial_edge</t>
+          <t>considered_axial_edge_count</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_intensity_outlier</t>
+          <t>considered_intensity_outlier_count</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_bad_z_fit</t>
+          <t>considered_bad_z_fit_count</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_bad_y_fit</t>
+          <t>considered_bad_y_fit_count</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>nr_of_beads_considered_bad_x_fit</t>
+          <t>considered_bad_x_fit_count</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>intensity_max_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>intensity_max_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>intensity_max_std</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>intensity_min_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>intensity_min_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>intensity_min_std</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>intensity_std_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>intensity_std_median</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>intensity_std_std</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>fit_r2_z_mean</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>fit_r2_z_median</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>fit_r2_z_std</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>fit_r2_y_mean</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>fit_r2_y_median</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>fit_r2_y_std</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>fit_r2_x_mean</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>fit_r2_x_median</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>fit_r2_x_std</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_z_pixels</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_y_pixels</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>resolution_mean_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>resolution_median_fwhm_x_pixels</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>resolution_std_fwhm_x_pixels</t>
-        </is>
-      </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_z_microns</t>
+          <t>fwhm_pixel_z_mean</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_z_microns</t>
+          <t>fwhm_pixel_z_median</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>resolution_std_fwhm_z_microns</t>
+          <t>fwhm_pixel_z_std</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_y_microns</t>
+          <t>fwhm_pixel_y_mean</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_y_microns</t>
+          <t>fwhm_pixel_y_median</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>resolution_std_fwhm_y_microns</t>
+          <t>fwhm_pixel_y_std</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_x_microns</t>
+          <t>fwhm_pixel_x_mean</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_x_microns</t>
+          <t>fwhm_pixel_x_median</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>resolution_std_fwhm_x_microns</t>
+          <t>fwhm_pixel_x_std</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>resolution_mean_fwhm_lateral_asymmetry_ratio</t>
+          <t>fwhm_micron_z_mean</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>resolution_median_fwhm_lateral_asymmetry_ratio</t>
+          <t>fwhm_micron_z_median</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>resolution_std_fwhm_lateral_asymmetry_ratio</t>
+          <t>fwhm_micron_z_std</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
+          <t>fwhm_micron_y_mean</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_median</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_std</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_mean</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_median</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_std</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_mean</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_median</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_std</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>column_series</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
           <t>data_reference</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>linked_references</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Merged with dev and deployed
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2354,12 +2354,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>discarded_bead_centers_lateral_edge</t>
+          <t>considered_bead_centers_lateral_edge</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>discarded_bead_centers_self_proximity</t>
+          <t>considered_bead_centers_self_proximity</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">

</xml_diff>

<commit_message>
renamed considered_bad_y_fit_count to considered_bad_fit_y_count and other dims
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2717,17 +2717,17 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>considered_bad_z_fit_count</t>
+          <t>considered_bad_fit_z_count</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>considered_bad_y_fit_count</t>
+          <t>considered_bad_fit_y_count</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>considered_bad_x_fit_count</t>
+          <t>considered_bad_fit_x_count</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">

</xml_diff>

<commit_message>
Replaced KeuValue for KeyMeasurements in FI schema
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -36,7 +36,7 @@
     <sheet name="FieldIlluminationDataset" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="FieldIlluminationInput" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="FieldIlluminationOutput" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="FieldIlluminationKeyValues" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="FieldIlluminationKeyMeasurements" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="PSFBeadsDataset" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="PSFBeadsInput" sheetId="32" state="visible" r:id="rId32"/>
     <sheet name="PSFBeadsOutput" sheetId="33" state="visible" r:id="rId33"/>
@@ -1740,7 +1740,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>key_values</t>
+          <t>key_measurements</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">

</xml_diff>

<commit_message>
renamed bead_x_profiles to bead_profiles_x
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2330,17 +2330,17 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>bead_z_profiles</t>
+          <t>bead_profiles_z</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>bead_y_profiles</t>
+          <t>bead_profiles_y</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>bead_x_profiles</t>
+          <t>bead_profiles_x</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">

</xml_diff>

<commit_message>
Added a table_data field to KeyMeasurements to store the tabular data object
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -1871,7 +1871,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2092,654 +2092,664 @@
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
           <t>data_reference</t>
         </is>
       </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>min_lateral_distance_factor</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fitting_r2_threshold</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>intensity_robust_z_score_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_self_proximity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_axial_edge</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_profiles_z</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_profiles_y</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_profiles_x</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>average_bead</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BN1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>considered_valid_count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_self_proximity_count</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_lateral_edge_count</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_axial_edge_count</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_intensity_outlier_count</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_z_count</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_y_count</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_x_count</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>intensity_max_mean</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>intensity_max_median</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>intensity_max_std</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>intensity_min_mean</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>intensity_min_median</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>intensity_min_std</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>intensity_std_mean</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>intensity_std_median</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>intensity_std_std</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_mean</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_median</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_std</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_mean</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_median</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_std</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_mean</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_median</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_std</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_mean</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_median</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_std</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_median</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_std</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_mean</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_median</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_std</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_median</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_std</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_mean</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_median</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_std</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_mean</t>
+        </is>
+      </c>
       <c r="AR1" t="inlineStr">
         <is>
+          <t>fwhm_micron_x_median</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_std</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_mean</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_median</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_std</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_z</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_y</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_x</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_z</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_y</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_x</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_z</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_y</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_x</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_max</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_min</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_std</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
           <t>linked_references</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fitting_r2_threshold</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>intensity_robust_z_score_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centers</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_self_proximity</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_axial_edge</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_z_fit_quality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_y_fit_quality</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_x_fit_quality</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>bead_properties</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>bead_profiles_z</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>bead_profiles_y</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>bead_profiles_x</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>average_bead</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BM1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_valid_count</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_self_proximity_count</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_lateral_edge_count</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_axial_edge_count</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_intensity_outlier_count</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_z_count</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_y_count</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_x_count</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>intensity_max_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>intensity_max_median</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>intensity_max_std</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>intensity_min_mean</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>intensity_min_median</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>intensity_min_std</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>intensity_std_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>intensity_std_median</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>intensity_std_std</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_mean</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_median</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_std</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_mean</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_median</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_std</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_median</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_std</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_mean</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_median</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_std</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_median</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_std</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_mean</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_median</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_std</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_median</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_std</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_mean</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_median</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_std</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_mean</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_median</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_std</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_mean</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_median</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_std</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_z</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_y</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_x</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_z</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_y</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_x</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_z</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_y</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_x</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_max</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_min</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_std</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Adding channel_name to PSFs for adding to key_measurements
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -839,7 +839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -860,10 +860,20 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1871,7 +1881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX1"/>
+  <dimension ref="A1:AY1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1902,889 +1912,899 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>channel_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>center_region_intensity_fraction</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y_relative</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x_relative</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>center_of_mass_distance_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>center_geometric_y</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>center_geometric_y_relative</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>center_geometric_x</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>center_geometric_x_relative</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>center_geometric_distance_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>center_fitted_y</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>center_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>center_fitted_x</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>center_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>center_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>center_region_area_fraction</t>
+          <t>acquisition_datetime</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>center_of_mass_y</t>
+          <t>processed</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>center_of_mass_y_relative</t>
+          <t>data_reference</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>center_of_mass_x</t>
+          <t>linked_references</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>center_of_mass_x_relative</t>
+          <t>name</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>center_of_mass_distance_relative</t>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>min_lateral_distance_factor</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fitting_r2_threshold</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>intensity_robust_z_score_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_self_proximity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_axial_edge</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_profiles_z</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>center_geometric_y</t>
+          <t>bead_profiles_y</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>center_geometric_y_relative</t>
+          <t>bead_profiles_x</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>center_geometric_x</t>
+          <t>average_bead</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>center_geometric_x_relative</t>
+          <t>processing_application</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>center_geometric_distance_relative</t>
+          <t>processing_version</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>center_fitted_y</t>
+          <t>processing_entity</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>center_fitted_y_relative</t>
+          <t>processing_datetime</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>center_fitted_x</t>
+          <t>processing_log</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>center_fitted_x_relative</t>
+          <t>warnings</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>center_fitted_distance_relative</t>
+          <t>errors</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>max_intensity</t>
+          <t>validated</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_y</t>
+          <t>validation_datetime</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_y_relative</t>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BS1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_valid_count</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_self_proximity_count</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_lateral_edge_count</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_axial_edge_count</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_intensity_outlier_count</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_z_count</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_y_count</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_x_count</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_mean</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_median</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_std</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>intensity_max_mean</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>intensity_max_median</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>intensity_max_std</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>intensity_min_mean</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>intensity_min_median</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>intensity_min_std</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>intensity_std_mean</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>intensity_std_median</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>intensity_std_std</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_mean</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_median</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_x</t>
+          <t>fit_r2_z_std</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_x_relative</t>
+          <t>fit_r2_y_mean</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>max_intensity_distance_relative</t>
+          <t>fit_r2_y_median</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>top_left_intensity_mean</t>
+          <t>fit_r2_y_std</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>top_left_intensity_ratio</t>
+          <t>fit_r2_x_mean</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>top_center_intensity_mean</t>
+          <t>fit_r2_x_median</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>top_center_intensity_ratio</t>
+          <t>fit_r2_x_std</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>top_right_intensity_mean</t>
+          <t>fwhm_pixel_z_mean</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>top_right_intensity_ratio</t>
+          <t>fwhm_pixel_z_median</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>middle_left_intensity_mean</t>
+          <t>fwhm_pixel_z_std</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>middle_left_intensity_ratio</t>
+          <t>fwhm_pixel_y_mean</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>middle_center_intensity_mean</t>
+          <t>fwhm_pixel_y_median</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>middle_center_intensity_ratio</t>
+          <t>fwhm_pixel_y_std</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>middle_right_intensity_mean</t>
+          <t>fwhm_pixel_x_mean</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>middle_right_intensity_ratio</t>
+          <t>fwhm_pixel_x_median</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>bottom_left_intensity_mean</t>
+          <t>fwhm_pixel_x_std</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>bottom_left_intensity_ratio</t>
+          <t>fwhm_micron_z_mean</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>bottom_center_intensity_mean</t>
+          <t>fwhm_micron_z_median</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>bottom_center_intensity_ratio</t>
+          <t>fwhm_micron_z_std</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>bottom_right_intensity_mean</t>
+          <t>fwhm_micron_y_mean</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>bottom_right_intensity_ratio</t>
+          <t>fwhm_micron_y_median</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
+          <t>fwhm_micron_y_std</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_mean</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_median</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_std</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_mean</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_median</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_std</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_z</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_y</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_x</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_z</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_y</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_x</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_z</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_y</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_x</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_integrated</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_max</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_min</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_std</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
           <t>table_data</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>data_reference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>linked_references</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fitting_r2_threshold</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>intensity_robust_z_score_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centers</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_self_proximity</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_axial_edge</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_z_fit_quality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_y_fit_quality</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_x_fit_quality</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>bead_properties</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>bead_profiles_z</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>bead_profiles_y</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>bead_profiles_x</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>average_bead</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BR1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_valid_count</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_self_proximity_count</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_lateral_edge_count</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_axial_edge_count</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_intensity_outlier_count</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_z_count</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_y_count</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_x_count</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_mean</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_median</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_std</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>intensity_max_mean</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>intensity_max_median</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>intensity_max_std</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>intensity_min_mean</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>intensity_min_median</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>intensity_min_std</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>intensity_std_mean</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>intensity_std_median</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>intensity_std_std</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_mean</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_median</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_std</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_mean</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_median</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_std</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_mean</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_median</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_std</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_median</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_std</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_mean</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_median</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_std</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_median</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_std</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_mean</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_median</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_std</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_mean</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_median</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_std</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_mean</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_median</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_std</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_mean</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_median</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_std</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_z</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_y</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_x</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_z</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_y</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_x</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_z</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_y</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_x</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_integrated</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_max</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_min</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_std</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Moved manufacturer to sample superclass Made use of slot_usage to specify allowed samples per dataset
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -32,31 +32,31 @@
     <sheet name="Vertex" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="Mask" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="Color" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="FieldIlluminationDataset" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="FieldIlluminationInputData" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="FieldIlluminationInputParameters" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="FieldIlluminationOutput" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="FieldIlluminationKeyMeasurements" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="PSFBeadsDataset" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="PSFBeadsInputData" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="PSFBeadsInputParameters" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="PSFBeadsOutput" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="PSFBeadsKeyMeasurements" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="ArgolightBDataset" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="ArgolightBInputData" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="ArgolightBInputParameters" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="ArgolightBOutput" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="ArgolightBCentersOfMass" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="ArgolightBIntensityKeyValues" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="ArgolightBDistanceKeyValues" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="ArgolightEDataset" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="ArgolightEInputData" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="ArgolightEInputParameters" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="ArgolightEOutput" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="ArgolightEKeyValues" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="FluorescentHomogeneousThickField" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet name="FluorescentHomogeneousThinField" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet name="PSFBeads" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="FluorescentHomogeneousThickField" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="FluorescentHomogeneousThinField" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="FieldIlluminationDataset" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="FieldIlluminationInputData" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="FieldIlluminationInputParameters" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="FieldIlluminationOutput" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="FieldIlluminationKeyMeasurements" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="PSFBeads" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="PSFBeadsDataset" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PSFBeadsInputData" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="PSFBeadsInputParameters" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="PSFBeadsOutput" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="PSFBeadsKeyMeasurements" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="ArgolightBDataset" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="ArgolightBInputData" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="ArgolightBInputParameters" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="ArgolightBOutput" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="ArgolightBCentersOfMass" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="ArgolightBIntensityKeyValues" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="ArgolightBDistanceKeyValues" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="ArgolightEDataset" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="ArgolightEInputData" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="ArgolightEInputParameters" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="ArgolightEOutput" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="ArgolightEKeyValues" sheetId="50" state="visible" r:id="rId50"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1577,6 +1577,88 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1652,7 +1734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1678,7 +1760,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>microscopes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1719,7 +1827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1835,7 +1943,410 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>image_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>image_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>channel_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y_relative</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x_relative</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>center_of_mass_distance_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>center_geometric_y</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>center_geometric_y_relative</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>center_geometric_x</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>center_geometric_x_relative</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>center_geometric_distance_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>center_fitted_y</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>center_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>center_fitted_x</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>center_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>center_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_diameter_micron</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1852,281 +2363,588 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>microscopes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>image_name</t>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>image_id</t>
+          <t>saturation_threshold</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>min_lateral_distance_factor</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fitting_r2_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>intensity_robust_z_score_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_self_proximity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_axial_edge</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_profiles_z</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_profiles_y</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_profiles_x</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>average_bead</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BS1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>channel_name</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_valid_count</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>channel_nr</t>
+          <t>considered_self_proximity_count</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>channel_id</t>
+          <t>considered_lateral_edge_count</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>center_region_intensity_fraction</t>
+          <t>considered_axial_edge_count</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>center_region_area_fraction</t>
+          <t>considered_intensity_outlier_count</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>center_of_mass_y</t>
+          <t>considered_bad_fit_z_count</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>center_of_mass_y_relative</t>
+          <t>considered_bad_fit_y_count</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>center_of_mass_x</t>
+          <t>considered_bad_fit_x_count</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>center_of_mass_x_relative</t>
+          <t>intensity_integrated_mean</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>center_of_mass_distance_relative</t>
+          <t>intensity_integrated_median</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>center_geometric_y</t>
+          <t>intensity_integrated_std</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>center_geometric_y_relative</t>
+          <t>intensity_max_mean</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>center_geometric_x</t>
+          <t>intensity_max_median</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>center_geometric_x_relative</t>
+          <t>intensity_max_std</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>center_geometric_distance_relative</t>
+          <t>intensity_min_mean</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>center_fitted_y</t>
+          <t>intensity_min_median</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>center_fitted_y_relative</t>
+          <t>intensity_min_std</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>center_fitted_x</t>
+          <t>intensity_std_mean</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>center_fitted_x_relative</t>
+          <t>intensity_std_median</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>center_fitted_distance_relative</t>
+          <t>intensity_std_std</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>max_intensity</t>
+          <t>fit_r2_z_mean</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_y</t>
+          <t>fit_r2_z_median</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_y_relative</t>
+          <t>fit_r2_z_std</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_x</t>
+          <t>fit_r2_y_mean</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>max_intensity_pos_x_relative</t>
+          <t>fit_r2_y_median</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>max_intensity_distance_relative</t>
+          <t>fit_r2_y_std</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>top_left_intensity_mean</t>
+          <t>fit_r2_x_mean</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>top_left_intensity_ratio</t>
+          <t>fit_r2_x_median</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>top_center_intensity_mean</t>
+          <t>fit_r2_x_std</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>top_center_intensity_ratio</t>
+          <t>fwhm_pixel_z_mean</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>top_right_intensity_mean</t>
+          <t>fwhm_pixel_z_median</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>top_right_intensity_ratio</t>
+          <t>fwhm_pixel_z_std</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>middle_left_intensity_mean</t>
+          <t>fwhm_pixel_y_mean</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>middle_left_intensity_ratio</t>
+          <t>fwhm_pixel_y_median</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>middle_center_intensity_mean</t>
+          <t>fwhm_pixel_y_std</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>middle_center_intensity_ratio</t>
+          <t>fwhm_pixel_x_mean</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>middle_right_intensity_mean</t>
+          <t>fwhm_pixel_x_median</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>middle_right_intensity_ratio</t>
+          <t>fwhm_pixel_x_std</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>bottom_left_intensity_mean</t>
+          <t>fwhm_micron_z_mean</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>bottom_left_intensity_ratio</t>
+          <t>fwhm_micron_z_median</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>bottom_center_intensity_mean</t>
+          <t>fwhm_micron_z_std</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>bottom_center_intensity_ratio</t>
+          <t>fwhm_micron_y_mean</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>bottom_right_intensity_mean</t>
+          <t>fwhm_micron_y_median</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>bottom_right_intensity_ratio</t>
+          <t>fwhm_micron_y_std</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
+          <t>fwhm_micron_x_mean</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_median</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_std</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_mean</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_median</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_std</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_z</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_y</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_x</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_z</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_y</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_x</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_z</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_y</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_x</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_integrated</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_max</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_min</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_std</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
           <t>table_data</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>data_reference</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>linked_references</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -2137,7 +2955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2210,889 +3028,6 @@
       <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>fitting_r2_threshold</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>intensity_robust_z_score_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centers</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_self_proximity</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_axial_edge</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_z_fit_quality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_y_fit_quality</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_x_fit_quality</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>bead_properties</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>bead_profiles_z</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>bead_profiles_y</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>bead_profiles_x</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>average_bead</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BS1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_valid_count</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_self_proximity_count</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_lateral_edge_count</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_axial_edge_count</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_intensity_outlier_count</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_z_count</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_y_count</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_x_count</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_mean</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_median</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_std</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>intensity_max_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>intensity_max_median</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>intensity_max_std</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>intensity_min_mean</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>intensity_min_median</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>intensity_min_std</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>intensity_std_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>intensity_std_median</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>intensity_std_std</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_mean</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_median</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_std</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_mean</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_median</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_std</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_median</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_std</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_mean</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_median</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_std</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_median</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_std</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_mean</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_median</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_std</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_median</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_std</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_mean</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_median</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_std</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_mean</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_median</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_std</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_mean</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_median</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_std</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_z</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_y</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_x</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_z</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_y</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_x</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_z</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_y</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_x</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_integrated</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_max</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_min</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_std</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="BS1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>argolight_b_image</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>spots_distance</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>lower_threshold_correction_factors</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>upper_threshold_correction_factors</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>remove_center_cross</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>spots_labels_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>spots_centers_of_mass</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>intensity_key_values</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>distance_key_values</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>spots_properties</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>spots_distances</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>comment</t>
         </is>
       </c>
     </row>
@@ -3178,6 +3113,199 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>argolight_b_image</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>spots_distance</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>lower_threshold_correction_factors</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>upper_threshold_correction_factors</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>remove_center_cross</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>spots_labels_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>spots_centers_of_mass</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>intensity_key_values</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>distance_key_values</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>spots_properties</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>spots_distances</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3243,7 +3371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3339,7 +3467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3430,7 +3558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3511,7 +3639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3537,7 +3665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3583,7 +3711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3669,7 +3797,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3750,170 +3924,6 @@
         </is>
       </c>
       <c r="N1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bead_diameter_micron</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Made sample a slot so that it can be used with slot_usage
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -491,12 +491,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>microscope</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sample</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -1685,14 +1685,626 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>microscope</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_image</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>microscopes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>roi_centers_of_mass</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centers_geometric</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>roi_centers_fitted</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>roi_centers_max_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>roi_center_region</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>image_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>image_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>channel_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y_relative</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x_relative</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>center_of_mass_distance_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>center_geometric_y</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>center_geometric_y_relative</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>center_geometric_x</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>center_geometric_x_relative</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>center_geometric_distance_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>center_fitted_y</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>center_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>center_fitted_x</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>center_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>center_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_diameter_micron</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>sample</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
           <t>experimenter</t>
@@ -1734,7 +2346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1751,48 +2363,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>field_illumination_image</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>microscopes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1813,1186 +2399,600 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>corner_fraction</t>
+          <t>min_lateral_distance_factor</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>sigma</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fitting_r2_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>intensity_robust_z_score_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_self_proximity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_axial_edge</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>key_measurements</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_profiles_z</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_profiles_y</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_profiles_x</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>average_bead</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BS1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>intensity_profiles</t>
+          <t>channel_nr</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>roi_profiles</t>
+          <t>considered_valid_count</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>roi_corners</t>
+          <t>considered_self_proximity_count</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>roi_centers_of_mass</t>
+          <t>considered_lateral_edge_count</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>roi_centers_geometric</t>
+          <t>considered_axial_edge_count</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>roi_centers_fitted</t>
+          <t>considered_intensity_outlier_count</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>roi_centers_max_intensity</t>
+          <t>considered_bad_fit_z_count</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>roi_center_region</t>
+          <t>considered_bad_fit_y_count</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>processing_application</t>
+          <t>considered_bad_fit_x_count</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>processing_version</t>
+          <t>intensity_integrated_mean</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>processing_entity</t>
+          <t>intensity_integrated_median</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>processing_datetime</t>
+          <t>intensity_integrated_std</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>processing_log</t>
+          <t>intensity_max_mean</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>warnings</t>
+          <t>intensity_max_median</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>errors</t>
+          <t>intensity_max_std</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>validated</t>
+          <t>intensity_min_mean</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>validation_datetime</t>
+          <t>intensity_min_median</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>image_name</t>
+          <t>intensity_min_std</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>intensity_std_mean</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>intensity_std_median</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>intensity_std_std</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_mean</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_median</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_std</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_mean</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_median</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_std</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_median</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_std</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_mean</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_median</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_std</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_median</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_std</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_mean</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_median</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_std</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_median</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_std</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_mean</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_median</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_std</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_mean</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_median</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_std</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_mean</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_median</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_std</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_z</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_y</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_x</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_z</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_y</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_x</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_z</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_y</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_x</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_integrated</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_max</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_min</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_std</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="BP1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="BQ1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="BR1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="BS1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>image_id</t>
+          <t>input_parameters</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>channel_name</t>
+          <t>output</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>channel_nr</t>
+          <t>sample</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>channel_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y_relative</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x_relative</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>center_of_mass_distance_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>center_geometric_y</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>center_geometric_y_relative</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>center_geometric_x</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>center_geometric_x_relative</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>center_geometric_distance_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>center_fitted_y</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>center_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>center_fitted_x</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>center_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>center_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bead_diameter_micron</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>microscope</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>fitting_r2_threshold</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>intensity_robust_z_score_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centers</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_self_proximity</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_axial_edge</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_z_fit_quality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_y_fit_quality</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_x_fit_quality</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>bead_properties</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>bead_profiles_z</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>bead_profiles_y</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>bead_profiles_x</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>average_bead</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BS1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_valid_count</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_self_proximity_count</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_lateral_edge_count</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_axial_edge_count</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_intensity_outlier_count</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_z_count</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_y_count</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_x_count</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_mean</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_median</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_std</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>intensity_max_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>intensity_max_median</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>intensity_max_std</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>intensity_min_mean</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>intensity_min_median</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>intensity_min_std</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>intensity_std_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>intensity_std_median</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>intensity_std_std</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_mean</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_median</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_std</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_mean</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_median</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_std</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_median</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_std</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_mean</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_median</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_std</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_median</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_std</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_mean</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_median</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_std</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_median</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_std</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_mean</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_median</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_std</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_mean</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_median</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_std</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_mean</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_median</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_std</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_z</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_y</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_x</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_z</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_y</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_x</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_z</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_y</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_x</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_integrated</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_max</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_min</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_std</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="BS1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sample</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -3590,12 +3590,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>microscope</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sample</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">

</xml_diff>

<commit_message>
Specifying sample range for psf_beads_schema.yaml
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -36,14 +36,14 @@
     <sheet name="FieldIlluminationInputParameters" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="FieldIlluminationOutput" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="FieldIlluminationKeyMeasurements" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="PSFBeadsDataset" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="PSFBeadsInputData" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="PSFBeadsInputParameters" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="PSFBeadsOutput" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="PSFBeadsKeyMeasurements" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="FluorescentHomogeneousThickField" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="FluorescentHomogeneousThinField" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="PSFBeads" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="PSFBeads" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="PSFBeadsDataset" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="PSFBeadsInputData" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="PSFBeadsInputParameters" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="PSFBeadsOutput" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PSFBeadsKeyMeasurements" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="FluorescentHomogeneousThickField" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="FluorescentHomogeneousThinField" sheetId="37" state="visible" r:id="rId37"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2049,6 +2049,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_diameter_micron</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2124,7 +2170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2150,7 +2196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2216,7 +2262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2357,7 +2403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2733,7 +2779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2774,7 +2820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2805,52 +2851,6 @@
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bead_diameter_micron</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Specifying sample range for field_illumination_schema.yaml
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -31,19 +31,19 @@
     <sheet name="Vertex" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="Mask" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="Color" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="FieldIlluminationDataset" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="FieldIlluminationInputData" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="FieldIlluminationInputParameters" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="FieldIlluminationOutput" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="FieldIlluminationKeyMeasurements" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="PSFBeads" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="PSFBeadsDataset" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="PSFBeadsInputData" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="PSFBeadsInputParameters" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="PSFBeadsOutput" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="PSFBeadsKeyMeasurements" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="FluorescentHomogeneousThickField" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="FluorescentHomogeneousThinField" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="FluorescentHomogeneousThickField" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="FluorescentHomogeneousThinField" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="FieldIlluminationDataset" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="FieldIlluminationInputData" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="FieldIlluminationInputParameters" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="FieldIlluminationOutput" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="FieldIlluminationKeyMeasurements" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="PSFBeads" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="PSFBeadsDataset" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="PSFBeadsInputData" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PSFBeadsInputParameters" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="PSFBeadsOutput" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="PSFBeadsKeyMeasurements" sheetId="37" state="visible" r:id="rId37"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1483,6 +1483,88 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1558,7 +1640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1584,7 +1666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1625,7 +1707,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>microscopes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1741,7 +1849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2017,7 +2125,134 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_diameter_micron</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2034,823 +2269,588 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>microscopes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bead_diameter_micron</t>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>protocol</t>
+          <t>saturation_threshold</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>manufacturer</t>
+          <t>min_lateral_distance_factor</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>sigma_z</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fitting_r2_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>intensity_robust_z_score_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_self_proximity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_axial_edge</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_profiles_z</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_profiles_y</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_profiles_x</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>average_bead</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BS1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_valid_count</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_self_proximity_count</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_lateral_edge_count</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_axial_edge_count</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_intensity_outlier_count</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_z_count</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_y_count</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_x_count</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_mean</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_median</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_std</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>intensity_max_mean</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>intensity_max_median</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>intensity_max_std</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>intensity_min_mean</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>intensity_min_median</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>intensity_min_std</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>intensity_std_mean</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>intensity_std_median</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>intensity_std_std</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_mean</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_median</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_std</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_mean</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_median</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_std</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_median</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_std</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_mean</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_median</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_std</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_median</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_std</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_mean</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_median</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_std</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_median</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_std</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_mean</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_median</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_std</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_mean</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_median</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_std</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_mean</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_median</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_std</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_z</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_y</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_x</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_z</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_y</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_x</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_z</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_y</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_x</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_integrated</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_max</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_min</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_std</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="BP1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="BQ1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="BR1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>fitting_r2_threshold</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>intensity_robust_z_score_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centers</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_self_proximity</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_axial_edge</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_z_fit_quality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_y_fit_quality</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_x_fit_quality</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>bead_properties</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>bead_profiles_z</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>bead_profiles_y</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>bead_profiles_x</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>average_bead</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BS1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_valid_count</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_self_proximity_count</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_lateral_edge_count</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_axial_edge_count</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_intensity_outlier_count</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_z_count</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_y_count</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_x_count</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_mean</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_median</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_std</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>intensity_max_mean</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>intensity_max_median</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>intensity_max_std</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>intensity_min_mean</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>intensity_min_median</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>intensity_min_std</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>intensity_std_mean</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>intensity_std_median</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>intensity_std_std</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_mean</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_median</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_std</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_mean</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_median</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_std</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_median</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_std</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_mean</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_median</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_std</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_median</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_std</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_mean</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_median</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_std</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_median</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_std</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_mean</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_median</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_std</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_mean</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_median</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_std</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_mean</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_median</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_std</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_z</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_y</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_x</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_z</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_y</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_x</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_z</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_y</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_x</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_integrated</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_max</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_min</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_std</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
       <c r="BS1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Made Experimenter and Comment Metrics objects
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2984,7 +2984,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3003,6 +3003,21 @@
           <t>orcid</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3015,7 +3030,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3042,6 +3057,26 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>text</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Renamed operational to user_experiment and iporting schema Other minor fixes
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PSFBeads" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="UserExperiment" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="MetaObject" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="DataReference" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="MicroscopeCollection" sheetId="4" state="visible" r:id="rId4"/>
@@ -32,18 +32,24 @@
     <sheet name="Vertex" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="Mask" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="Color" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="FluorescentHomogeneousThickField" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="FluorescentHomogeneousThinField" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="PSFBeadsDataset" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="PSFBeadsInputData" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="PSFBeadsInputParameters" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="PSFBeadsOutput" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="PSFBeadsKeyMeasurements" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="FieldIlluminationDataset" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="FieldIlluminationInputData" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="FieldIlluminationInputParameters" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="FieldIlluminationOutput" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="FieldIlluminationKeyMeasurements" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="PSFBeads" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="FluorescentHomogeneousThickField" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="FluorescentHomogeneousThinField" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="UserExperimentDataset" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="UserExperimentInputData" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="UserExperimentInputParameters" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="UserExperimentOutput" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="UserExperimentKeyMeasurements" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="PSFBeadsDataset" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PSFBeadsInputData" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="PSFBeadsInputParameters" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="PSFBeadsOutput" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="PSFBeadsKeyMeasurements" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="FieldIlluminationDataset" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="FieldIlluminationInputData" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="FieldIlluminationInputParameters" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="FieldIlluminationOutput" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="FieldIlluminationKeyMeasurements" sheetId="43" state="visible" r:id="rId43"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,6 +455,413 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dataset_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>datasets</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>voxel_size_x_micron</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>voxel_size_y_micron</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>voxel_size_z_micron</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>shape_x</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>shape_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>shape_z</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>shape_c</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>shape_t</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>time_series</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>channel_series</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>source_images</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>array_data</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>voxel_size_x_micron</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>voxel_size_y_micron</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>voxel_size_z_micron</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>shape_x</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>shape_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>shape_z</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>shape_c</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>shape_t</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>time_series</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>channel_series</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>source_images</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>array_data</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channels</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>excitation_wavelength_nm</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>emission_wavelength_nm</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -460,6 +873,674 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>source_reference</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>data_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>values</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>points</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>lines</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rectangles</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ellipses</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>polygons</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>masks</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fill_color</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>stroke_color</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>stroke_width</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>y1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>x2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>y2</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fill_color</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>stroke_color</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>stroke_width</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fill_color</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>stroke_color</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>stroke_width</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>x_rad</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>y_rad</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fill_color</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>stroke_color</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>stroke_width</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>vertexes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>is_open</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fill_color</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>stroke_color</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>stroke_width</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mask</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>fill_color</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>stroke_color</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>stroke_width</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>alpha</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>bead_diameter_micron</t>
         </is>
       </c>
@@ -489,1221 +1570,161 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>dataset_class</t>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>datasets</t>
+          <t>manufacturer</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>data_reference</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>linked_references</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>voxel_size_x_micron</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>voxel_size_y_micron</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>voxel_size_z_micron</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>shape_x</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>shape_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>shape_z</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>shape_c</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>shape_t</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>time_series</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>channel_series</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>source_images</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>array_data</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>voxel_size_x_micron</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>voxel_size_y_micron</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>voxel_size_z_micron</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>shape_x</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>shape_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>shape_z</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>shape_c</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>shape_t</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>time_series</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>channel_series</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>source_images</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>array_data</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channels</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>excitation_wavelength_nm</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>emission_wavelength_nm</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>values</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>source_reference</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>data_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>values</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>points</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>lines</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rectangles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ellipses</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>polygons</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>masks</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>fill_color</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>stroke_color</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>stroke_width</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>y1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>x2</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>fill_color</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>stroke_color</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>stroke_width</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>w</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>fill_color</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>stroke_color</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>stroke_width</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>x_rad</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>y_rad</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>fill_color</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>stroke_color</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>stroke_width</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>vertexes</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>is_open</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>fill_color</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>stroke_color</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>stroke_width</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mask</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>fill_color</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>stroke_color</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>stroke_width</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>alpha</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
         </is>
       </c>
     </row>
@@ -1769,6 +1790,319 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>user_experiment_images</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orthogonal_rois</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>profile_rois</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orthogonal_images</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fft_images</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>variation_coefficient</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1829,7 +2163,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1970,7 +2304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2346,7 +2680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2427,7 +2761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2444,6 +2778,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>microscopes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>field_illumination_image</t>
         </is>
       </c>
@@ -2453,7 +2813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2494,7 +2854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2610,7 +2970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2878,32 +3238,6 @@
       <c r="AY1" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>microscopes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added orthogonal images to core schema and to user_experiment_schema.yaml
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -19,37 +19,38 @@
     <sheet name="HarmonizedMetricsDatasetCollection" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Image" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="ImageMask" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="ChannelSeries" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Channel" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="TimeSeries" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Column" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Roi" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Point" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Line" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Rectangle" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="Ellipse" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Polygon" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="Vertex" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Mask" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="Color" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="PSFBeads" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="FluorescentHomogeneousThickField" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="FluorescentHomogeneousThinField" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="UserExperimentDataset" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="UserExperimentInputData" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="UserExperimentInputParameters" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="UserExperimentOutput" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="UserExperimentKeyMeasurements" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="PSFBeadsDataset" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="PSFBeadsInputData" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="PSFBeadsInputParameters" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="PSFBeadsOutput" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="PSFBeadsKeyMeasurements" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="FieldIlluminationDataset" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="FieldIlluminationInputData" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="FieldIlluminationInputParameters" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="FieldIlluminationOutput" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="FieldIlluminationKeyMeasurements" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="OrthogonalImage" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="ChannelSeries" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Channel" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="TimeSeries" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Column" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Roi" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Point" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Line" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Rectangle" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Ellipse" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Polygon" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Vertex" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Mask" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Color" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="PSFBeads" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="FluorescentHomogeneousThickField" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="FluorescentHomogeneousThinField" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="UserExperimentDataset" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="UserExperimentInputData" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="UserExperimentInputParameters" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="UserExperimentOutput" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="UserExperimentKeyMeasurements" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PSFBeadsDataset" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="PSFBeadsInputData" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="PSFBeadsInputParameters" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="PSFBeadsOutput" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="PSFBeadsKeyMeasurements" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="FieldIlluminationDataset" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="FieldIlluminationInputData" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="FieldIlluminationInputParameters" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="FieldIlluminationOutput" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="FieldIlluminationKeyMeasurements" sheetId="44" state="visible" r:id="rId44"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -759,6 +760,132 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>source_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source_roi</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>axis</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>voxel_size_x_micron</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>voxel_size_y_micron</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>voxel_size_z_micron</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>shape_x</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>shape_y</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>shape_z</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>shape_c</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>shape_t</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>time_series</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>channel_series</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>source_images</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>array_data</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"XY,XZ,YZ"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -779,7 +906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -830,7 +957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -856,7 +983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -902,7 +1029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -973,7 +1100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1044,7 +1171,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1125,25 +1270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1224,7 +1351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1305,7 +1432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1376,7 +1503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1407,7 +1534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1483,7 +1610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1524,7 +1651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1570,7 +1697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1611,7 +1738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1642,87 +1769,6 @@
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1790,6 +1836,87 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1820,7 +1947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1838,7 +1965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1929,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1995,7 +2122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2076,7 +2203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2102,7 +2229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2168,7 +2295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2309,7 +2436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2685,7 +2812,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>microscopes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2766,7 +2919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2783,32 +2936,6 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>microscopes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>field_illumination_image</t>
         </is>
       </c>
@@ -2818,7 +2945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2859,7 +2986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2975,7 +3102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Removed source image from orthogonal image as already contained in image superclass. Removed wrong if_absent value
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -686,119 +686,114 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>source_image</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>source_roi</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>axis</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>axis</t>
+          <t>voxel_size_x_micron</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>voxel_size_x_micron</t>
+          <t>voxel_size_y_micron</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>voxel_size_y_micron</t>
+          <t>voxel_size_z_micron</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>voxel_size_z_micron</t>
+          <t>shape_x</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>shape_x</t>
+          <t>shape_y</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>shape_y</t>
+          <t>shape_z</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>shape_z</t>
+          <t>shape_c</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>shape_c</t>
+          <t>shape_t</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>shape_t</t>
+          <t>time_series</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>time_series</t>
+          <t>channel_series</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>channel_series</t>
+          <t>acquisition_datetime</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>acquisition_datetime</t>
+          <t>source_images</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>source_images</t>
+          <t>array_data</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>array_data</t>
+          <t>data_reference</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>data_reference</t>
+          <t>linked_references</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>linked_references</t>
+          <t>name</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"XY,XZ,YZ"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3351,7 +3346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3377,25 +3372,30 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>saturated_channels</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>table_data</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>data_reference</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>linked_references</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Initial commit of light_source_power
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -45,12 +45,24 @@
     <sheet name="PSFBeadsInputParameters" sheetId="36" state="visible" r:id="rId36"/>
     <sheet name="PSFBeadsOutput" sheetId="37" state="visible" r:id="rId37"/>
     <sheet name="PSFBeadsKeyMeasurements" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="UserExperiment" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="UserExperimentDataset" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="UserExperimentInputData" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="UserExperimentInputParameters" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="UserExperimentOutput" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="UserExperimentKeyMeasurements" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="LightSourcePowerDataset" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="SimpleLightSourcePowerDataset" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="LightSourcePowerInputData" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="LightSourcePowerInputParameters" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="LightSourcePowerOutput" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="SimpleLightSourcePowerOutput" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="LightSourcePowerKeyMeasurements" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="SimpleLightSourcePowerKeyMeasurements" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="PowerSample" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="LightSource" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="PowerMeter" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="UserExperiment" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="UserExperimentDataset" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="UserExperimentInputData" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="UserExperimentInputParameters" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet name="UserExperimentOutput" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet name="UserExperimentKeyMeasurements" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet name="LightSourcePower" sheetId="56" state="visible" r:id="rId56"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2995,31 +3007,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -3188,6 +3240,344 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>measurement_device</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>power_samples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>light_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>power_mean_mw</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>power_median_mw</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>power_std_mw</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>power_min_mw</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>power_max_mw</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>linearity</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>light_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>power_mw</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3199,6 +3589,277 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>light_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sampling_datetime</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>power_mw</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>wavelength_nm</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>user_experiment_images</t>
         </is>
       </c>
@@ -3218,7 +3879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3249,7 +3910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3340,7 +4001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3406,42 +4067,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>url</t>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Added a key_measurement to track the total nr of beads detected
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -2638,7 +2638,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BS1"/>
+  <dimension ref="A1:BT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2659,345 +2659,350 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>total_bead_count</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>considered_valid_count</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>considered_self_proximity_count</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>considered_lateral_edge_count</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>considered_axial_edge_count</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>considered_intensity_outlier_count</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>considered_bad_fit_z_count</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>considered_bad_fit_y_count</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>considered_bad_fit_x_count</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>intensity_integrated_mean</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>intensity_integrated_median</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>intensity_integrated_std</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>intensity_max_mean</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>intensity_max_median</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>intensity_max_std</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>intensity_min_mean</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>intensity_min_median</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>intensity_min_std</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>intensity_std_mean</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>intensity_std_median</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>intensity_std_std</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>fit_r2_z_mean</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>fit_r2_z_median</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>fit_r2_z_std</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>fit_r2_y_mean</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>fit_r2_y_median</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>fit_r2_y_std</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>fit_r2_x_mean</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>fit_r2_x_median</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>fit_r2_x_std</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>fwhm_pixel_z_mean</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>fwhm_pixel_z_median</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>fwhm_pixel_z_std</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>fwhm_pixel_y_mean</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>fwhm_pixel_y_median</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>fwhm_pixel_y_std</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>fwhm_pixel_x_mean</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>fwhm_pixel_x_median</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>fwhm_pixel_x_std</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>fwhm_micron_z_mean</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>fwhm_micron_z_median</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>fwhm_micron_z_std</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>fwhm_micron_y_mean</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>fwhm_micron_y_median</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>fwhm_micron_y_std</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>fwhm_micron_x_mean</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>fwhm_micron_x_median</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>fwhm_micron_x_std</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>fwhm_lateral_asymmetry_ratio_mean</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>fwhm_lateral_asymmetry_ratio_median</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>fwhm_lateral_asymmetry_ratio_std</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>average_bead_fit_r2_z</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>average_bead_fit_r2_y</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>average_bead_fit_r2_x</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>average_bead_fwhm_pixel_z</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>average_bead_fwhm_pixel_y</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>average_bead_fwhm_pixel_x</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>average_bead_fwhm_micron_z</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>average_bead_fwhm_micron_y</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>average_bead_fwhm_micron_x</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>average_bead_intensity_integrated</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>average_bead_intensity_max</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>average_bead_intensity_min</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>average_bead_intensity_std</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>table_data</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>data_reference</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>linked_references</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Minor changes to Light power
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -3301,7 +3301,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3317,61 +3317,56 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>power_set_point_pct</t>
+          <t>power_mean_mw</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>power_mean_mw</t>
+          <t>power_median_mw</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>power_median_mw</t>
+          <t>power_std_mw</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>power_std_mw</t>
+          <t>power_min_mw</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>power_min_mw</t>
+          <t>power_max_mw</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>power_max_mw</t>
+          <t>linearity</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>linearity</t>
+          <t>table_data</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>table_data</t>
+          <t>data_reference</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>data_reference</t>
+          <t>linked_references</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>linked_references</t>
+          <t>name</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
           <t>description</t>
         </is>
       </c>
@@ -3387,32 +3382,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>light_source</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sampling_datetime</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>sampling_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>power_set_point</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>power_mw</t>
         </is>
       </c>
-    </row>
-  </sheetData>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>integration_time_ms</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"SOURCE_EXIT,FIBER_EXIT,OBJECTIVE_BACKFOCAL,OBJECTIVE_EXIT,OBJECTIVE_FOCAL,OTHER"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Made Mixins for datasets that Have Sample and Have Input Parameters. Adapted strategies, test data and tests accordingly
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -53,7 +53,13 @@
     <sheet name="PowerSample" sheetId="44" state="visible" r:id="rId44"/>
     <sheet name="LightSource" sheetId="45" state="visible" r:id="rId45"/>
     <sheet name="PowerMeter" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="LightSourcePower" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="UserExperiment" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="UserExperimentDataset" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="UserExperimentInputData" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="UserExperimentInputParameters" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="UserExperimentOutput" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="UserExperimentKeyMeasurements" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="LightSourcePower" sheetId="53" state="visible" r:id="rId53"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1707,1382 +1713,1372 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>acquisition_datetime</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>acquisition_protocol</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>field_illumination_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>microscope_collection</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>corner_fraction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>intensity_profiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>roi_profiles</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>roi_corners</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>roi_centers_of_mass</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>roi_centers_geometric</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>roi_centers_fitted</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>roi_centers_max_intensity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>roi_center_region</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>image_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>image_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>channel_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>center_region_intensity_fraction</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>center_region_area_fraction</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>center_of_mass_y_relative</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>center_of_mass_x_relative</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>center_of_mass_distance_relative</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>center_geometric_y</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>center_geometric_y_relative</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>center_geometric_x</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>center_geometric_x_relative</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>center_geometric_distance_relative</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>center_fitted_y</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>center_fitted_y_relative</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>center_fitted_x</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>center_fitted_x_relative</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>center_fitted_distance_relative</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>max_intensity</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_y_relative</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>max_intensity_pos_x_relative</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>max_intensity_distance_relative</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>top_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>top_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>top_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>middle_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>middle_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>middle_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>bottom_left_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>bottom_center_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_mean</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>bottom_right_intensity_ratio</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bead_diameter_micron</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>preparation_protocol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>input_data</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>acquisition_protocol</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>psf_beads_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>min_lateral_distance_factor</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>input_parameters</t>
+          <t>sigma_z</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>sigma_y</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sigma_x</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>snr_threshold</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>fitting_r2_threshold</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>intensity_robust_z_score_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>analyzed_bead_centers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_lateral_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_self_proximity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_axial_edge</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_intensity_outlier</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_z_fit_quality</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_y_fit_quality</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_bead_centers_x_fit_quality</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bead_properties</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bead_profiles_z</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>bead_profiles_y</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>bead_profiles_x</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>average_bead</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BT1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>total_bead_count</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>considered_valid_count</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>considered_self_proximity_count</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>considered_lateral_edge_count</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>considered_axial_edge_count</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>considered_intensity_outlier_count</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_z_count</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_y_count</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>considered_bad_fit_x_count</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_mean</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_median</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>intensity_integrated_std</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>intensity_max_mean</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>intensity_max_median</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>intensity_max_std</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>intensity_min_mean</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>intensity_min_median</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>intensity_min_std</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>intensity_std_mean</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>intensity_std_median</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>intensity_std_std</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_mean</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_median</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>fit_r2_z_std</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_mean</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_median</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>fit_r2_y_std</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_mean</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_median</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>fit_r2_x_std</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_mean</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_median</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_z_std</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_mean</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_median</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_y_std</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_mean</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_median</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>fwhm_pixel_x_std</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_mean</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_median</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_z_std</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_mean</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_median</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_y_std</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_mean</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_median</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>fwhm_micron_x_std</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_mean</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_median</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>fwhm_lateral_asymmetry_ratio_std</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_z</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_y</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>average_bead_fit_r2_x</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_z</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_y</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_pixel_x</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_z</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_y</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_micron_x</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_integrated</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_max</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_min</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
+          <t>average_bead_intensity_std</t>
+        </is>
+      </c>
+      <c r="BP1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="BQ1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="BR1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="BS1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="BT1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>output</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>microscope</t>
+          <t>acquisition_protocol</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>experimenter</t>
+          <t>processed</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>acquisition_protocol</t>
+          <t>data_reference</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>processed</t>
+          <t>linked_references</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>data_reference</t>
+          <t>name</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>field_illumination_images</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>microscope_collection</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>corner_fraction</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sigma</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>intensity_profiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>roi_profiles</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>roi_corners</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>roi_centers_of_mass</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>roi_centers_geometric</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>roi_centers_fitted</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>roi_centers_max_intensity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>roi_center_region</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>image_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>image_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>channel_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>center_region_intensity_fraction</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>center_region_area_fraction</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>center_of_mass_y_relative</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>center_of_mass_x_relative</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>center_of_mass_distance_relative</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>center_geometric_y</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>center_geometric_y_relative</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>center_geometric_x</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>center_geometric_x_relative</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>center_geometric_distance_relative</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>center_fitted_y</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>center_fitted_y_relative</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>center_fitted_x</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>center_fitted_x_relative</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>center_fitted_distance_relative</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>max_intensity</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_y_relative</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>max_intensity_pos_x_relative</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>max_intensity_distance_relative</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>top_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>top_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>top_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>middle_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>middle_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>middle_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>bottom_left_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>bottom_center_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_mean</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>bottom_right_intensity_ratio</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bead_diameter_micron</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>preparation_protocol</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>acquisition_protocol</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>psf_beads_images</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>min_lateral_distance_factor</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>sigma_z</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sigma_y</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sigma_x</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>snr_threshold</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>fitting_r2_threshold</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>intensity_robust_z_score_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:X1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>analyzed_bead_centers</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_lateral_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_self_proximity</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_axial_edge</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_intensity_outlier</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_z_fit_quality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_y_fit_quality</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_bead_centers_x_fit_quality</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>bead_properties</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>bead_profiles_z</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>bead_profiles_y</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>bead_profiles_x</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>average_bead</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BT1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>total_bead_count</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>considered_valid_count</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>considered_self_proximity_count</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>considered_lateral_edge_count</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>considered_axial_edge_count</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>considered_intensity_outlier_count</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_z_count</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_y_count</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>considered_bad_fit_x_count</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_mean</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_median</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>intensity_integrated_std</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>intensity_max_mean</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>intensity_max_median</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>intensity_max_std</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>intensity_min_mean</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>intensity_min_median</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>intensity_min_std</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>intensity_std_mean</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>intensity_std_median</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>intensity_std_std</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_mean</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_median</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>fit_r2_z_std</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_mean</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_median</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>fit_r2_y_std</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_mean</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_median</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>fit_r2_x_std</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_mean</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_median</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_z_std</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_mean</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_median</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_y_std</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_mean</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_median</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>fwhm_pixel_x_std</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_mean</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_median</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_z_std</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_mean</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_median</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_y_std</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_mean</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_median</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>fwhm_micron_x_std</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_mean</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_median</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>fwhm_lateral_asymmetry_ratio_std</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_z</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_y</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>average_bead_fit_r2_x</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_z</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_y</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_pixel_x</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_z</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_y</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_micron_x</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>average_bead_fwhm_lateral_asymmetry_ratio</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_integrated</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_max</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_min</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>average_bead_intensity_std</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="BS1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="BT1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>acquisition_datetime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input_data</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>acquisition_protocol</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -3534,6 +3530,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>input_parameters</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>acquisition_datetime</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input_data</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>microscope</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>experimenter</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>acquisition_protocol</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>user_experiment_images</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orthogonal_rois</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>profile_rois</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -3570,6 +3688,235 @@
         </is>
       </c>
       <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bit_depth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>saturation_threshold</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>intensity_profiles_b</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orthogonal_images</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fft_images</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>key_measurements</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>processing_application</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>processing_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>processing_entity</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>processing_datetime</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>processing_log</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>warnings</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>errors</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>validated</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>validation_datetime</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>channel_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>channel_nr</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>variation_coefficient</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>saturated_channels</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>table_data</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>data_reference</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>linked_references</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>preparation_protocol</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
Revert wrongfully assignment of ProfilesIntensity mixin to profile tables
</commit_message>
<xml_diff>
--- a/project/excel/microscopemetrics_schema.xlsx
+++ b/project/excel/microscopemetrics_schema.xlsx
@@ -53,13 +53,7 @@
     <sheet name="PowerSample" sheetId="44" state="visible" r:id="rId44"/>
     <sheet name="LightSource" sheetId="45" state="visible" r:id="rId45"/>
     <sheet name="PowerMeter" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="UserExperiment" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="UserExperimentDataset" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet name="UserExperimentInputData" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet name="UserExperimentInputParameters" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet name="UserExperimentOutput" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet name="UserExperimentKeyMeasurements" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet name="LightSourcePower" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet name="LightSourcePower" sheetId="47" state="visible" r:id="rId47"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3530,393 +3524,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>input_parameters</t>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>authors</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>acquisition_datetime</t>
+          <t>url</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>input_data</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>microscope</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>experimenter</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>acquisition_protocol</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processed</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>user_experiment_images</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>orthogonal_rois</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>profile_rois</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>bit_depth</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>saturation_threshold</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>intensity_profiles_b</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>orthogonal_images</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>fft_images</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>key_measurements</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>comment</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>processing_application</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>processing_version</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>processing_entity</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>processing_datetime</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>processing_log</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>warnings</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>errors</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>validated</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>validation_datetime</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>channel_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>channel_nr</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>variation_coefficient</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>saturated_channels</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>table_data</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>data_reference</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>linked_references</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>preparation_protocol</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>